<commit_message>
EPBDS-7870 SmartRules: CharRange is not supported in Smart Rules
--HG--
branch : 5.21.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7870_CharRangeTests.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7870_CharRangeTests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkamalov\.openl\user-workspace\DEFAULT\CharRangeTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191E09FA-8CAF-4071-A58A-1ECC817B387A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FAD426-4783-4776-8D25-C973D0838831}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="55">
   <si>
     <t>C1</t>
   </si>
@@ -164,6 +164,27 @@
   </si>
   <si>
     <t>Test getCharValueRule getCharValueRuleTest</t>
+  </si>
+  <si>
+    <t>A-D</t>
+  </si>
+  <si>
+    <t>M-Z</t>
+  </si>
+  <si>
+    <t>SmartLookup String getCharValueRule3(char value, char tier)</t>
+  </si>
+  <si>
+    <t>Test getCharValueRule3 getCharValueRule3Test</t>
+  </si>
+  <si>
+    <t>tier</t>
+  </si>
+  <si>
+    <t>Tier</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -295,7 +316,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -316,6 +337,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -662,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05770BFD-7FD0-474C-B875-B44EB075EE5E}">
-  <dimension ref="C4:D101"/>
+  <dimension ref="B4:E118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44:C53"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="K110" sqref="K110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,10 +710,10 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
@@ -793,10 +828,10 @@
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="10"/>
+      <c r="D23" s="16"/>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C24" s="5" t="s">
@@ -911,10 +946,10 @@
       </c>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D42" s="10"/>
+      <c r="D42" s="16"/>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C43" s="3" t="s">
@@ -1005,10 +1040,10 @@
       </c>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="8" t="s">
+      <c r="C57" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D57" s="8"/>
+      <c r="D57" s="14"/>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C58" s="7" t="s">
@@ -1107,10 +1142,10 @@
       </c>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C73" s="8" t="s">
+      <c r="C73" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D73" s="8"/>
+      <c r="D73" s="14"/>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C74" s="7" t="s">
@@ -1209,10 +1244,10 @@
       </c>
     </row>
     <row r="89" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C89" s="8" t="s">
+      <c r="C89" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D89" s="8"/>
+      <c r="D89" s="14"/>
     </row>
     <row r="90" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C90" s="7" t="s">
@@ -1270,7 +1305,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C97" s="7" t="s">
         <v>40</v>
       </c>
@@ -1278,7 +1313,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C98" s="7" t="s">
         <v>43</v>
       </c>
@@ -1286,7 +1321,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C99" s="7" t="s">
         <v>33</v>
       </c>
@@ -1294,7 +1329,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C100" s="7" t="s">
         <v>42</v>
       </c>
@@ -1302,7 +1337,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C101" s="7" t="s">
         <v>41</v>
       </c>
@@ -1310,8 +1345,131 @@
         <v>22</v>
       </c>
     </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C105" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D105" s="12"/>
+      <c r="E105" s="12"/>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C106" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D106" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E106" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C107" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D107" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B108" s="8"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B109" s="8"/>
+      <c r="C109" s="8"/>
+      <c r="D109" s="8"/>
+      <c r="E109" s="8"/>
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B110" s="8"/>
+      <c r="C110" s="8"/>
+      <c r="D110" s="8"/>
+      <c r="E110" s="8"/>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B111" s="8"/>
+      <c r="C111" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D111" s="13"/>
+      <c r="E111" s="13"/>
+    </row>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B112" s="8"/>
+      <c r="C112" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D112" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E112" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B113" s="8"/>
+      <c r="C113" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D113" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E113" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B114" s="8"/>
+      <c r="C114" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D114" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E114" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B115" s="8"/>
+      <c r="C115" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D115" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E115" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B116" s="8"/>
+      <c r="C116" s="8"/>
+      <c r="D116" s="8"/>
+      <c r="E116" s="8"/>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B117" s="8"/>
+      <c r="C117" s="8"/>
+      <c r="D117" s="8"/>
+      <c r="E117" s="8"/>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B118" s="8"/>
+      <c r="C118" s="8"/>
+      <c r="D118" s="8"/>
+      <c r="E118" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="C105:E105"/>
+    <mergeCell ref="C111:E111"/>
     <mergeCell ref="C73:D73"/>
     <mergeCell ref="C89:D89"/>
     <mergeCell ref="C4:D4"/>

</xml_diff>